<commit_message>
update SQAP in SPMP and code line tracker
</commit_message>
<xml_diff>
--- a/docs/code line tracker.xlsx
+++ b/docs/code line tracker.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cs673\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="135" windowWidth="19395" windowHeight="7605" activeTab="8"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
   <si>
     <t>Code lines tracker</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,23 +58,27 @@
   <si>
     <t>Algorithm</t>
   </si>
+  <si>
+    <t>Yike Xue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -88,7 +87,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -128,7 +127,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,7 +143,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -186,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,14 +435,14 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -471,7 +470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -481,7 +480,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -491,7 +490,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -501,7 +500,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -511,7 +510,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -521,7 +520,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -531,7 +530,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -541,7 +540,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -551,7 +550,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -561,7 +560,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -571,7 +570,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -581,7 +580,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -601,14 +600,14 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -636,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -646,7 +645,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -656,7 +655,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -666,7 +665,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -676,7 +675,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -686,7 +685,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -696,7 +695,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -706,7 +705,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -716,7 +715,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -726,7 +725,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -736,7 +735,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -746,7 +745,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -766,14 +765,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -781,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -801,7 +800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -811,7 +810,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -821,7 +820,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -831,7 +830,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -841,7 +840,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -851,7 +850,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -861,7 +860,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -871,7 +870,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -881,7 +880,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -891,7 +890,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -901,7 +900,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -911,7 +910,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -931,14 +930,14 @@
       <selection activeCell="B25" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -966,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -976,7 +975,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -986,7 +985,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1006,7 +1005,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1016,7 +1015,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1026,7 +1025,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1036,7 +1035,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1046,7 +1045,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1056,7 +1055,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1066,7 +1065,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1076,7 +1075,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1093,17 +1092,17 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1141,7 +1140,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1151,7 +1150,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1161,7 +1160,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1171,7 +1170,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1181,7 +1180,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1191,7 +1190,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1201,7 +1200,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1211,7 +1210,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1221,7 +1220,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1231,7 +1230,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1241,7 +1240,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1258,17 +1257,17 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1306,7 +1305,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1316,7 +1315,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1326,7 +1325,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1336,17 +1335,21 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1">
+        <v>149</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1356,7 +1359,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1376,7 +1379,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1386,7 +1389,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1396,7 +1399,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1406,7 +1409,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1426,14 +1429,14 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1471,7 +1474,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1481,7 +1484,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1491,7 +1494,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1501,7 +1504,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1511,7 +1514,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1521,7 +1524,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1531,7 +1534,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1541,7 +1544,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1551,7 +1554,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1561,7 +1564,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1571,7 +1574,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1591,14 +1594,15 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1629,7 +1633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1639,7 +1643,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1649,7 +1653,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1659,7 +1663,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1669,7 +1673,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1682,7 +1686,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1692,7 +1696,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1702,7 +1706,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1712,7 +1716,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1722,7 +1726,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1732,7 +1736,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1742,7 +1746,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1759,25 +1763,28 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1797,7 +1804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1807,17 +1814,19 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>163</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1829,7 +1838,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1837,7 +1846,7 @@
         <v>299</v>
       </c>
       <c r="C7" s="1">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
@@ -1845,17 +1854,21 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>160</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>78</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1865,7 +1878,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1875,7 +1888,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1885,7 +1898,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1895,7 +1908,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1905,7 +1918,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1915,7 +1928,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Fixed add visit problem and roughly add current visit page
</commit_message>
<xml_diff>
--- a/docs/code line tracker.xlsx
+++ b/docs/code line tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="140" windowWidth="19400" windowHeight="7600" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="144" windowWidth="19404" windowHeight="7596"/>
   </bookViews>
   <sheets>
     <sheet name="Allen" sheetId="11" r:id="rId1"/>
@@ -71,8 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,7 +132,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -431,17 +431,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -531,8 +531,12 @@
         <v>6</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1">
+        <v>32</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
@@ -604,17 +608,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -773,17 +777,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -942,17 +946,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1111,17 +1115,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1280,17 +1284,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1457,17 +1461,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1626,17 +1630,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1802,17 +1806,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>